<commit_message>
added new files; replaced bad symbols; added a new description
</commit_message>
<xml_diff>
--- a/evenki_texts_corpus_desc.xlsx
+++ b/evenki_texts_corpus_desc.xlsx
@@ -1,271 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="11475" windowHeight="6975"/>
-  </bookViews>
-  <sheets>
-    <sheet name="evenki_texts" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="125725" refMode="R1C1"/>
-</workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="83">
-  <si>
-    <t>2006_Ozero_Bolshoe_Sovetskoe_Saygotin_LO2_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2006_Ozero_Bolshoe_Sovetskoe_Saygotin_LO3_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FM10_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FM1_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FM2_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FM5_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FM7_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FM8_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FSk10_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FSk2_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FSk3_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FSk6_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_FSk9_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Ekonda_Kombagir_Anna_LR1_2_transliterated_transliterated2.eaf</t>
-  </si>
-  <si>
-    <t>2007_Ekonda_Udygir_Viktor_FSk3_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2007_Vanavara_Torpushonok_LO.eaf</t>
-  </si>
-  <si>
-    <t>2008_Tura_Eldygir_Liliya_LAv_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2008_Tura_Eldygir_Liliya_LR1_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2008_Tura_Lapuko_LR3_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2008_Tutonchany_Khukochar_Danil_LR_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2011_Hantayskoye_Ozero_Chempogir_Antonina_Dmitriyevna_LB1_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2011_Hantayskoye_Ozero_Chempogir_Antonina_Dmitriyevna_LR.eaf</t>
-  </si>
-  <si>
-    <t>2011_Hantayskoye_Ozero_Turskaya_Minna_Dmitriyevna_LR1_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2011_Hantayskoye_Ozero_Turskaya_Minna_Dmitriyevna_L_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2011_Hantayskoye_Ozero_Yeryomina_Lyubov_LR_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2011_Potapovo_Bogdanova_Tamara_Andreevna_FM1_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2014_Tura_Eldogir_EK_LR1_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>2014_Uchami_Mukto_Stalina_LB3_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>Arch_Lebedeva_1952_Uchami_Bukharev_BearCub_new.eaf</t>
-  </si>
-  <si>
-    <t>Arch_Lebedeva_1952_Uchami_Bukharov_Summer_transliterated.eaf</t>
-  </si>
-  <si>
-    <t>Arch_Levedeva_1952_Tura_Uvachan_Cannibals.eaf</t>
-  </si>
-  <si>
-    <t>Arch_Levedeva_1952_Tutonchany_Yalogir_Chulugdy.eaf</t>
-  </si>
-  <si>
-    <t>Arch_Levedeva_1952_Uchami_Lopoko_Robbery.eaf</t>
-  </si>
-  <si>
-    <t>имя файла</t>
-  </si>
-  <si>
-    <t>место записи</t>
-  </si>
-  <si>
-    <t>дата записи</t>
-  </si>
-  <si>
-    <t>информант</t>
-  </si>
-  <si>
-    <t>полевая расшифровка</t>
-  </si>
-  <si>
-    <t>архивный</t>
-  </si>
-  <si>
-    <t>Большое Советское Озеро</t>
-  </si>
-  <si>
-    <t>Чиринда</t>
-  </si>
-  <si>
-    <t>Эконда</t>
-  </si>
-  <si>
-    <t>Ванавара</t>
-  </si>
-  <si>
-    <t>Тура</t>
-  </si>
-  <si>
-    <t>Тутончаны</t>
-  </si>
-  <si>
-    <t>Хантайское Озеро</t>
-  </si>
-  <si>
-    <t>Потапово</t>
-  </si>
-  <si>
-    <t>Учами</t>
-  </si>
-  <si>
-    <t>Сайготин Владимир Николаевич</t>
-  </si>
-  <si>
-    <t>Елдогир Валентина Христофоровна</t>
-  </si>
-  <si>
-    <t>Комбагир Анна Николаевна, Удыгир Изольда Николаевна</t>
-  </si>
-  <si>
-    <t>Удыгир Виктор Николаевич</t>
-  </si>
-  <si>
-    <t>Торпушонок Татьяна Ивановна</t>
-  </si>
-  <si>
-    <t>Елдогир Лилия Михайловна</t>
-  </si>
-  <si>
-    <t>Хукочар Данил Афанасьевич</t>
-  </si>
-  <si>
-    <t>Чемпогир Антонина Дмитриевна</t>
-  </si>
-  <si>
-    <t>Турская Минна(Зинаида) Дмитриевна</t>
-  </si>
-  <si>
-    <t>Еремина Любовь Алексеевна, Турская Минна(Зинаида) Дмитриевна</t>
-  </si>
-  <si>
-    <t>Богданова Тамара Андреевна</t>
-  </si>
-  <si>
-    <t>Эспек (Елдогир) Елена Кирилловна</t>
-  </si>
-  <si>
-    <t>Мукто Сталина Прокопьевна</t>
-  </si>
-  <si>
-    <t>Казакевич О. А.</t>
-  </si>
-  <si>
-    <t>морфологический анализ</t>
-  </si>
-  <si>
-    <t>Мамонтова Н. А.</t>
-  </si>
-  <si>
-    <t>Клячко Е. Л.</t>
-  </si>
-  <si>
-    <t>Лебедева Е. П.</t>
-  </si>
-  <si>
-    <t>Митрофанова Н. К.</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>Бухарев Вениамин</t>
-  </si>
-  <si>
-    <t>Увачан Ира</t>
-  </si>
-  <si>
-    <t>Ялогир Тамара</t>
-  </si>
-  <si>
-    <t>Лопоко Нина</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_LR1.eaf_new.eaf</t>
-  </si>
-  <si>
-    <t>2007_Chirinda_Eldogir_Valentina_LR2Ev.eaf_new.eaf</t>
-  </si>
-  <si>
-    <t>2007_Ekonda_Khutokogir_Grigoriy_LAv.eaf_new.eaf</t>
-  </si>
-  <si>
-    <t>Хутокогир Григорий Николаевич</t>
-  </si>
-  <si>
-    <t>2007_Ekonda_Pankagir_LAv_transliterated.eaf_new.eaf</t>
-  </si>
-  <si>
-    <t>Панкагир Антон Никитич</t>
-  </si>
-  <si>
-    <t>2008_Kislokan_Udygir_Valentina_LAv.eaf_new.eaf</t>
-  </si>
-  <si>
-    <t>Кислокан</t>
-  </si>
-  <si>
-    <t>Удыгир Валентина Иннокентьевна</t>
-  </si>
-  <si>
-    <t>2008_Kislokan_Udygir_Valentina_LR1.eaf_new.eaf</t>
-  </si>
-  <si>
-    <t>2008_Kislokan_Udygir_Valentina_LR2.eaf_new.eaf</t>
-  </si>
-</sst>
-</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">

</xml_diff>